<commit_message>
Latest Automation Test Scripts
LAA added
</commit_message>
<xml_diff>
--- a/src/com/data/Test Cases Laa.xlsx
+++ b/src/com/data/Test Cases Laa.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="78">
   <si>
     <t>TCID</t>
   </si>
@@ -71,25 +71,184 @@
     <t>BOILERSOIL@GMAIL.COM :: Oil Work :: New Installation :: Oil Work</t>
   </si>
   <si>
-    <t>LaaOilBurner</t>
-  </si>
-  <si>
-    <t>LAA Oil Burner Installer</t>
-  </si>
-  <si>
     <t>DOBTEST05@GMAIL.COM :: Fire Suppression Work :: New Installation :: Equipment</t>
   </si>
   <si>
-    <t xml:space="preserve">LAA Fire Suppression Contractor </t>
-  </si>
-  <si>
     <t>Laa :: BOILERPLUMBER@GMAIL.COM :: Master Plumber :: THE PLUMBING COMPANY INC</t>
   </si>
   <si>
-    <t>LaaFireSuppression</t>
-  </si>
-  <si>
     <t>BOILERPLUMBER@GMAIL.COM :: Gas Plumbing Work :: New Installation :: Gas Work</t>
+  </si>
+  <si>
+    <t>legalization :: true :: exempt</t>
+  </si>
+  <si>
+    <t>exempt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LAA - Legalization Violation 'Yes' with  Number </t>
+  </si>
+  <si>
+    <t>LAA - Legalization Violation 'No'</t>
+  </si>
+  <si>
+    <t>legalization :: false :: exempt</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>FireSuppressionPay</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fire Suppression Pay </t>
+  </si>
+  <si>
+    <t>pay_now</t>
+  </si>
+  <si>
+    <t>BOILERPLUMBER@GMAIL.COM :: check</t>
+  </si>
+  <si>
+    <t>BOILERPLUMBER@GMAIL.COM</t>
+  </si>
+  <si>
+    <t>DOBTEST05@GMAIL.COM</t>
+  </si>
+  <si>
+    <t>BOILERSOIL@GMAIL.COM</t>
+  </si>
+  <si>
+    <t>BOILERPLUMBER@GMAIL.COM :: Water Plumbing Work :: New Installation :: Water Piping</t>
+  </si>
+  <si>
+    <t>Boiler Gas Exempt</t>
+  </si>
+  <si>
+    <t>PlumbingGas</t>
+  </si>
+  <si>
+    <t>PlumbingGasPay</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plumbing Gas Pay </t>
+  </si>
+  <si>
+    <t>PlumbingWaterPay</t>
+  </si>
+  <si>
+    <t>PlumbingWater</t>
+  </si>
+  <si>
+    <t>Plumbing Water Exempt</t>
+  </si>
+  <si>
+    <t>Plumbing Water Pay</t>
+  </si>
+  <si>
+    <t>OilBurnerPay</t>
+  </si>
+  <si>
+    <t>OilBurner</t>
+  </si>
+  <si>
+    <t>Oil Burner Exempt</t>
+  </si>
+  <si>
+    <t>Oil Burner Pay</t>
+  </si>
+  <si>
+    <t>BOILERSOIL@GMAIL.COM :: check</t>
+  </si>
+  <si>
+    <t>FireSuppression</t>
+  </si>
+  <si>
+    <t>DOBTEST05@GMAIL.COM :: Fire Suppression Work :: New Installation :: Fire Suppression Work</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Fire Suppression Exempt</t>
+  </si>
+  <si>
+    <t>DOBTEST05@GMAIL.COM :: check</t>
+  </si>
+  <si>
+    <t>LegalizationNo</t>
+  </si>
+  <si>
+    <t>LegalizationYes</t>
+  </si>
+  <si>
+    <t>Equipment</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Equipment - Appliance Data mandatory </t>
+  </si>
+  <si>
+    <t>PaaOnPermitted</t>
+  </si>
+  <si>
+    <t>action</t>
+  </si>
+  <si>
+    <t>PAA on permitted</t>
+  </si>
+  <si>
+    <t>paa</t>
+  </si>
+  <si>
+    <t>EwnFromDash</t>
+  </si>
+  <si>
+    <t>LaaFromEwn</t>
+  </si>
+  <si>
+    <t>LAA from EWN</t>
+  </si>
+  <si>
+    <t>Create LAA</t>
+  </si>
+  <si>
+    <t>EWN from dashboard + EWN</t>
+  </si>
+  <si>
+    <t>PAA on Permitted – Corrections Requested</t>
+  </si>
+  <si>
+    <t>DOBTEST05@GMAIL.COM :: Permitted – Corrections Requested :: exempt :: PAA</t>
+  </si>
+  <si>
+    <t>DOBTEST05@GMAIL.COM :: Permitted :: exempt :: PAA</t>
+  </si>
+  <si>
+    <t>PaaOnCorrerctions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LAA with scope of work without Appliance Data </t>
+  </si>
+  <si>
+    <t>WithoutAppliance</t>
+  </si>
+  <si>
+    <t>EwnNumber</t>
+  </si>
+  <si>
+    <t>ewn</t>
+  </si>
+  <si>
+    <t>CommerciaWhirlpool</t>
+  </si>
+  <si>
+    <t>Commercia Whirlpool</t>
+  </si>
+  <si>
+    <t>BOILERPLUMBER@GMAIL.COM :: Water Plumbing Work :: New Installation :: Fixture</t>
+  </si>
+  <si>
+    <t>exempt :: Commercial</t>
+  </si>
+  <si>
+    <t>Construction Code Determination Form (CCD1)</t>
   </si>
 </sst>
 </file>
@@ -1435,10 +1594,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:C30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="32.85546875" defaultRowHeight="12.75"/>
@@ -1460,141 +1619,176 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" s="2" customFormat="1">
       <c r="A2" s="27" t="s">
-        <v>23</v>
-      </c>
+        <v>73</v>
+      </c>
+      <c r="B2" s="22"/>
       <c r="C2" s="24" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" s="2" customFormat="1">
       <c r="A3" s="27" t="s">
-        <v>10</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="B3" s="22"/>
       <c r="C3" s="24" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="27" t="s">
-        <v>18</v>
+        <v>60</v>
       </c>
       <c r="C4" s="24" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="20"/>
+    <row r="5" spans="1:3" s="2" customFormat="1">
+      <c r="A5" s="27" t="s">
+        <v>71</v>
+      </c>
+      <c r="B5" s="26"/>
       <c r="C5" s="24" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:3" s="2" customFormat="1">
-      <c r="A6" s="27"/>
-      <c r="B6" s="26"/>
+    <row r="6" spans="1:3">
+      <c r="A6" s="27" t="s">
+        <v>48</v>
+      </c>
       <c r="C6" s="24" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="27"/>
+    <row r="7" spans="1:3" s="2" customFormat="1">
+      <c r="A7" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="26"/>
       <c r="C7" s="24" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="27"/>
+      <c r="A8" s="27" t="s">
+        <v>61</v>
+      </c>
       <c r="C8" s="24" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="27"/>
+    <row r="9" spans="1:3" s="2" customFormat="1">
+      <c r="A9" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="B9" s="22"/>
       <c r="C9" s="24" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:3" s="2" customFormat="1">
-      <c r="A10" s="20"/>
-      <c r="B10" s="22"/>
+    <row r="10" spans="1:3">
+      <c r="A10" s="27" t="s">
+        <v>53</v>
+      </c>
       <c r="C10" s="24" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:3" s="2" customFormat="1">
-      <c r="A11" s="20"/>
-      <c r="B11" s="22"/>
+    <row r="11" spans="1:3">
+      <c r="A11" s="27" t="s">
+        <v>44</v>
+      </c>
       <c r="C11" s="24" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:3" s="2" customFormat="1">
-      <c r="A12" s="20"/>
-      <c r="B12" s="26"/>
+    <row r="12" spans="1:3">
+      <c r="A12" s="27" t="s">
+        <v>43</v>
+      </c>
       <c r="C12" s="24" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:3" s="2" customFormat="1">
-      <c r="A13" s="27"/>
-      <c r="B13" s="26"/>
+      <c r="A13" s="27" t="s">
+        <v>68</v>
+      </c>
+      <c r="B13" s="22"/>
       <c r="C13" s="24" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:3" s="2" customFormat="1">
-      <c r="A14" s="27"/>
+      <c r="A14" s="27" t="s">
+        <v>56</v>
+      </c>
       <c r="B14" s="26"/>
       <c r="C14" s="24" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:3" s="2" customFormat="1">
-      <c r="A15" s="27"/>
+      <c r="A15" s="27" t="s">
+        <v>36</v>
+      </c>
       <c r="B15" s="26"/>
       <c r="C15" s="24" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:3">
-      <c r="A16" s="27"/>
+      <c r="A16" s="27" t="s">
+        <v>37</v>
+      </c>
       <c r="C16" s="24" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:3">
-      <c r="A17" s="20"/>
+      <c r="A17" s="27" t="s">
+        <v>40</v>
+      </c>
       <c r="C17" s="24" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="18" spans="1:3">
-      <c r="A18" s="20"/>
+      <c r="A18" s="27" t="s">
+        <v>39</v>
+      </c>
       <c r="C18" s="24" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
-      <c r="A19" s="20"/>
+    <row r="19" spans="1:3" s="2" customFormat="1">
+      <c r="A19" s="27" t="s">
+        <v>70</v>
+      </c>
+      <c r="B19" s="22"/>
       <c r="C19" s="24" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
-      <c r="A20" s="20"/>
+    <row r="20" spans="1:3" s="2" customFormat="1">
+      <c r="A20" s="27"/>
+      <c r="B20" s="26"/>
       <c r="C20" s="24" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" s="2" customFormat="1">
       <c r="A21" s="27"/>
+      <c r="B21" s="26"/>
       <c r="C21" s="24" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" s="2" customFormat="1">
       <c r="A22" s="27"/>
+      <c r="B22" s="26"/>
       <c r="C22" s="24" t="s">
         <v>3</v>
       </c>
@@ -1606,14 +1800,44 @@
       </c>
     </row>
     <row r="24" spans="1:3">
-      <c r="A24" s="27"/>
+      <c r="A24" s="20"/>
       <c r="C24" s="24" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="25" spans="1:3">
-      <c r="A25" s="27"/>
+      <c r="A25" s="20"/>
       <c r="C25" s="24" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="27"/>
+      <c r="C26" s="24" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" s="27"/>
+      <c r="C27" s="24" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" s="27"/>
+      <c r="C28" s="24" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" s="27"/>
+      <c r="C29" s="24" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" s="27"/>
+      <c r="C30" s="24" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1625,25 +1849,27 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N13"/>
+  <dimension ref="A1:N77"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F21" sqref="F21"/>
+    <sheetView showFormulas="1" tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="F1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="35.28515625" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" style="8" customWidth="1"/>
+    <col min="1" max="1" width="9" style="8" customWidth="1"/>
     <col min="2" max="2" width="19.7109375" style="13" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="41.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" style="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="41.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.28515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="3.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="10" max="14" width="35.28515625" style="8"/>
+    <col min="3" max="3" width="19.140625" style="8" customWidth="1"/>
+    <col min="4" max="4" width="19.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.85546875" style="8" customWidth="1"/>
+    <col min="7" max="7" width="4.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.5703125" style="8" customWidth="1"/>
+    <col min="9" max="9" width="12.7109375" style="9" customWidth="1"/>
+    <col min="10" max="10" width="13.28515625" style="8" customWidth="1"/>
+    <col min="11" max="11" width="2" style="8" bestFit="1" customWidth="1"/>
+    <col min="12" max="14" width="35.28515625" style="8"/>
     <col min="15" max="16384" width="35.28515625" style="9"/>
   </cols>
   <sheetData>
@@ -1665,12 +1891,12 @@
     </row>
     <row r="2" spans="1:14" s="6" customFormat="1">
       <c r="A2" s="27" t="s">
-        <v>23</v>
+        <v>73</v>
       </c>
       <c r="B2" s="5"/>
       <c r="D2" s="5"/>
       <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
       <c r="J2" s="5"/>
       <c r="K2" s="5"/>
       <c r="L2" s="5"/>
@@ -1697,49 +1923,53 @@
         <v>16</v>
       </c>
       <c r="G3" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3" s="29" t="s">
         <v>5</v>
-      </c>
-      <c r="H3" s="29" t="s">
-        <v>8</v>
       </c>
       <c r="I3" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="J3" s="28"/>
+      <c r="J3" s="28" t="s">
+        <v>72</v>
+      </c>
       <c r="K3" s="28"/>
       <c r="L3" s="28"/>
       <c r="M3" s="28"/>
       <c r="N3" s="28"/>
     </row>
-    <row r="4" spans="1:14" s="4" customFormat="1" ht="25.5">
+    <row r="4" spans="1:14" s="4" customFormat="1" ht="39.75" customHeight="1">
       <c r="A4" s="19" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>21</v>
+        <v>74</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>14</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>3</v>
+        <v>76</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>24</v>
+        <v>75</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>3</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>3</v>
+        <v>77</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="J4" s="10"/>
+        <v>31</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>3</v>
+      </c>
       <c r="K4" s="10"/>
       <c r="L4" s="10"/>
       <c r="M4" s="10"/>
@@ -1766,12 +1996,12 @@
     </row>
     <row r="7" spans="1:14" s="6" customFormat="1">
       <c r="A7" s="27" t="s">
-        <v>10</v>
+        <v>54</v>
       </c>
       <c r="B7" s="5"/>
       <c r="D7" s="5"/>
       <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
       <c r="J7" s="5"/>
       <c r="K7" s="5"/>
       <c r="L7" s="5"/>
@@ -1798,10 +2028,10 @@
         <v>16</v>
       </c>
       <c r="G8" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="H8" s="29" t="s">
         <v>5</v>
-      </c>
-      <c r="H8" s="29" t="s">
-        <v>8</v>
       </c>
       <c r="I8" s="29" t="s">
         <v>9</v>
@@ -1817,7 +2047,7 @@
         <v>3</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>11</v>
+        <v>55</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>13</v>
@@ -1826,10 +2056,10 @@
         <v>14</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>3</v>
+        <v>22</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>3</v>
@@ -1838,7 +2068,7 @@
         <v>3</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>3</v>
+        <v>32</v>
       </c>
       <c r="J9" s="10"/>
       <c r="K9" s="10"/>
@@ -1846,90 +2076,1484 @@
       <c r="M9" s="10"/>
       <c r="N9" s="10"/>
     </row>
-    <row r="10" spans="1:14" s="6" customFormat="1">
-      <c r="A10" s="27" t="s">
+    <row r="10" spans="1:14">
+      <c r="A10" s="21"/>
+    </row>
+    <row r="11" spans="1:14" s="6" customFormat="1">
+      <c r="A11" s="27" t="s">
+        <v>60</v>
+      </c>
+      <c r="B11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="5"/>
+      <c r="M11" s="5"/>
+      <c r="N11" s="5"/>
+    </row>
+    <row r="12" spans="1:14" s="7" customFormat="1">
+      <c r="A12" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="E12" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="F12" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="G12" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="H12" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="I12" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="J12" s="28"/>
+      <c r="K12" s="28"/>
+      <c r="L12" s="28"/>
+      <c r="M12" s="28"/>
+      <c r="N12" s="28"/>
+    </row>
+    <row r="13" spans="1:14" s="4" customFormat="1" ht="25.5">
+      <c r="A13" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="J13" s="10"/>
+      <c r="K13" s="10"/>
+      <c r="L13" s="10"/>
+      <c r="M13" s="10"/>
+      <c r="N13" s="10"/>
+    </row>
+    <row r="14" spans="1:14">
+      <c r="A14" s="21"/>
+    </row>
+    <row r="15" spans="1:14" s="6" customFormat="1">
+      <c r="A15" s="27" t="s">
+        <v>71</v>
+      </c>
+      <c r="B15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="H15" s="5"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="5"/>
+      <c r="L15" s="5"/>
+      <c r="M15" s="5"/>
+      <c r="N15" s="5"/>
+    </row>
+    <row r="16" spans="1:14" s="7" customFormat="1">
+      <c r="A16" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="E16" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="F16" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="G16" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="H16" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="I16" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="J16" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="K16" s="28"/>
+      <c r="L16" s="28"/>
+      <c r="M16" s="28"/>
+      <c r="N16" s="28"/>
+    </row>
+    <row r="17" spans="1:14" s="4" customFormat="1" ht="25.5">
+      <c r="A17" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="I17" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="J17" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K17" s="10"/>
+      <c r="L17" s="10"/>
+      <c r="M17" s="10"/>
+      <c r="N17" s="10"/>
+    </row>
+    <row r="18" spans="1:14">
+      <c r="A18" s="21"/>
+    </row>
+    <row r="19" spans="1:14" s="6" customFormat="1">
+      <c r="A19" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="B19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="H19" s="5"/>
+      <c r="J19" s="5"/>
+      <c r="K19" s="5"/>
+      <c r="L19" s="5"/>
+      <c r="M19" s="5"/>
+      <c r="N19" s="5"/>
+    </row>
+    <row r="20" spans="1:14" s="7" customFormat="1">
+      <c r="A20" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C20" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="E20" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="F20" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="G20" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="H20" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="I20" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="J20" s="28"/>
+      <c r="K20" s="28"/>
+      <c r="L20" s="28"/>
+      <c r="M20" s="28"/>
+      <c r="N20" s="28"/>
+    </row>
+    <row r="21" spans="1:14" s="4" customFormat="1" ht="25.5">
+      <c r="A21" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="B21" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="H21" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="I21" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="J21" s="10"/>
+      <c r="K21" s="10"/>
+      <c r="L21" s="10"/>
+      <c r="M21" s="10"/>
+      <c r="N21" s="10"/>
+    </row>
+    <row r="22" spans="1:14">
+      <c r="A22" s="21"/>
+    </row>
+    <row r="23" spans="1:14" s="6" customFormat="1">
+      <c r="A23" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="B23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="H23" s="5"/>
+      <c r="J23" s="5"/>
+      <c r="K23" s="5"/>
+      <c r="L23" s="5"/>
+      <c r="M23" s="5"/>
+      <c r="N23" s="5"/>
+    </row>
+    <row r="24" spans="1:14" s="7" customFormat="1">
+      <c r="A24" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B24" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C24" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="D24" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="E24" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="F24" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="G24" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="H24" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="I24" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="J24" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="K24" s="28"/>
+      <c r="L24" s="28"/>
+      <c r="M24" s="28"/>
+      <c r="N24" s="28"/>
+    </row>
+    <row r="25" spans="1:14" s="4" customFormat="1" ht="25.5">
+      <c r="A25" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="B25" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="H25" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="I25" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="J25" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="K25" s="10"/>
+      <c r="L25" s="10"/>
+      <c r="M25" s="10"/>
+      <c r="N25" s="10"/>
+    </row>
+    <row r="27" spans="1:14" s="6" customFormat="1">
+      <c r="A27" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="B27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="F27" s="5"/>
+      <c r="H27" s="5"/>
+      <c r="J27" s="5"/>
+      <c r="K27" s="5"/>
+      <c r="L27" s="5"/>
+      <c r="M27" s="5"/>
+      <c r="N27" s="5"/>
+    </row>
+    <row r="28" spans="1:14" s="7" customFormat="1">
+      <c r="A28" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B28" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C28" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="D28" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="E28" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="F28" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="G28" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="H28" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="I28" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="J28" s="28" t="s">
+        <v>57</v>
+      </c>
+      <c r="K28" s="28"/>
+      <c r="L28" s="28"/>
+      <c r="M28" s="28"/>
+      <c r="N28" s="28"/>
+    </row>
+    <row r="29" spans="1:14" s="4" customFormat="1" ht="25.5">
+      <c r="A29" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="B29" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="G29" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="H29" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="I29" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="J29" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="K29" s="10"/>
+      <c r="L29" s="10"/>
+      <c r="M29" s="10"/>
+      <c r="N29" s="10"/>
+    </row>
+    <row r="30" spans="1:14">
+      <c r="A30" s="21"/>
+    </row>
+    <row r="31" spans="1:14" s="6" customFormat="1">
+      <c r="A31" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="B31" s="5"/>
+      <c r="D31" s="5"/>
+      <c r="F31" s="5"/>
+      <c r="H31" s="5"/>
+      <c r="J31" s="5"/>
+      <c r="K31" s="5"/>
+      <c r="L31" s="5"/>
+      <c r="M31" s="5"/>
+      <c r="N31" s="5"/>
+    </row>
+    <row r="32" spans="1:14" s="7" customFormat="1">
+      <c r="A32" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B32" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C32" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="D32" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="E32" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="F32" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="G32" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="H32" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="I32" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="J32" s="28"/>
+      <c r="K32" s="28"/>
+      <c r="L32" s="28"/>
+      <c r="M32" s="28"/>
+      <c r="N32" s="28"/>
+    </row>
+    <row r="33" spans="1:14" s="4" customFormat="1" ht="25.5">
+      <c r="A33" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="B33" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F33" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="G33" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="H33" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="I33" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="J33" s="10"/>
+      <c r="K33" s="10"/>
+      <c r="L33" s="10"/>
+      <c r="M33" s="10"/>
+      <c r="N33" s="10"/>
+    </row>
+    <row r="34" spans="1:14">
+      <c r="A34" s="21"/>
+    </row>
+    <row r="35" spans="1:14" s="6" customFormat="1">
+      <c r="A35" s="27" t="s">
+        <v>53</v>
+      </c>
+      <c r="B35" s="5"/>
+      <c r="D35" s="5"/>
+      <c r="F35" s="5"/>
+      <c r="H35" s="5"/>
+      <c r="J35" s="5"/>
+      <c r="K35" s="5"/>
+      <c r="L35" s="5"/>
+      <c r="M35" s="5"/>
+      <c r="N35" s="5"/>
+    </row>
+    <row r="36" spans="1:14" s="7" customFormat="1" ht="38.25">
+      <c r="A36" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B36" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C36" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="D36" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="E36" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="F36" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="G36" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="H36" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="I36" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="J36" s="28"/>
+      <c r="K36" s="28"/>
+      <c r="L36" s="28"/>
+      <c r="M36" s="28"/>
+      <c r="N36" s="28"/>
+    </row>
+    <row r="37" spans="1:14" s="4" customFormat="1" ht="25.5">
+      <c r="A37" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="B37" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F37" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="G37" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="H37" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="I37" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="J37" s="10"/>
+      <c r="K37" s="10"/>
+      <c r="L37" s="10"/>
+      <c r="M37" s="10"/>
+      <c r="N37" s="10"/>
+    </row>
+    <row r="38" spans="1:14">
+      <c r="A38" s="21"/>
+    </row>
+    <row r="39" spans="1:14" s="6" customFormat="1">
+      <c r="A39" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="B39" s="5"/>
+      <c r="D39" s="5"/>
+      <c r="F39" s="5"/>
+      <c r="H39" s="5"/>
+      <c r="J39" s="5"/>
+      <c r="K39" s="5"/>
+      <c r="L39" s="5"/>
+      <c r="M39" s="5"/>
+      <c r="N39" s="5"/>
+    </row>
+    <row r="40" spans="1:14" s="7" customFormat="1">
+      <c r="A40" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B40" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C40" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="D40" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="E40" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="F40" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="G40" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="H40" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="I40" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="J40" s="28"/>
+      <c r="K40" s="28"/>
+      <c r="L40" s="28"/>
+      <c r="M40" s="28"/>
+      <c r="N40" s="28"/>
+    </row>
+    <row r="41" spans="1:14" s="4" customFormat="1" ht="25.5">
+      <c r="A41" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="B41" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E41" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F41" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="G41" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="H41" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="I41" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="J41" s="10"/>
+      <c r="K41" s="10"/>
+      <c r="L41" s="10"/>
+      <c r="M41" s="10"/>
+      <c r="N41" s="10"/>
+    </row>
+    <row r="43" spans="1:14" s="6" customFormat="1">
+      <c r="A43" s="27" t="s">
+        <v>44</v>
+      </c>
+      <c r="B43" s="5"/>
+      <c r="D43" s="5"/>
+      <c r="F43" s="5"/>
+      <c r="H43" s="5"/>
+      <c r="J43" s="5"/>
+      <c r="K43" s="5"/>
+      <c r="L43" s="5"/>
+      <c r="M43" s="5"/>
+      <c r="N43" s="5"/>
+    </row>
+    <row r="44" spans="1:14" s="7" customFormat="1">
+      <c r="A44" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B44" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C44" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="D44" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="E44" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="F44" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="G44" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="H44" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="I44" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="J44" s="28"/>
+      <c r="K44" s="28"/>
+      <c r="L44" s="28"/>
+      <c r="M44" s="28"/>
+      <c r="N44" s="28"/>
+    </row>
+    <row r="45" spans="1:14" s="4" customFormat="1" ht="25.5">
+      <c r="A45" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="B45" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D45" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E45" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F45" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G45" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="H45" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="I45" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="J45" s="10"/>
+      <c r="K45" s="10"/>
+      <c r="L45" s="10"/>
+      <c r="M45" s="10"/>
+      <c r="N45" s="10"/>
+    </row>
+    <row r="46" spans="1:14">
+      <c r="A46" s="21"/>
+    </row>
+    <row r="47" spans="1:14" s="6" customFormat="1">
+      <c r="A47" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="B47" s="5"/>
+      <c r="D47" s="5"/>
+      <c r="F47" s="5"/>
+      <c r="H47" s="5"/>
+      <c r="J47" s="5"/>
+      <c r="K47" s="5"/>
+      <c r="L47" s="5"/>
+      <c r="M47" s="5"/>
+      <c r="N47" s="5"/>
+    </row>
+    <row r="48" spans="1:14" s="7" customFormat="1">
+      <c r="A48" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B48" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C48" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="D48" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="E48" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="F48" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="G48" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="H48" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="I48" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="J48" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="K48" s="28"/>
+      <c r="L48" s="28"/>
+      <c r="M48" s="28"/>
+      <c r="N48" s="28"/>
+    </row>
+    <row r="49" spans="1:14" s="4" customFormat="1" ht="25.5">
+      <c r="A49" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="B49" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D49" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E49" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F49" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G49" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="H49" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="I49" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="J49" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="K49" s="10"/>
+      <c r="L49" s="10"/>
+      <c r="M49" s="10"/>
+      <c r="N49" s="10"/>
+    </row>
+    <row r="50" spans="1:14">
+      <c r="A50" s="21"/>
+    </row>
+    <row r="51" spans="1:14" s="6" customFormat="1">
+      <c r="A51" s="27" t="s">
+        <v>68</v>
+      </c>
+      <c r="B51" s="5"/>
+      <c r="D51" s="5"/>
+      <c r="F51" s="5"/>
+      <c r="H51" s="5"/>
+      <c r="J51" s="5"/>
+      <c r="K51" s="5"/>
+      <c r="L51" s="5"/>
+      <c r="M51" s="5"/>
+      <c r="N51" s="5"/>
+    </row>
+    <row r="52" spans="1:14" s="7" customFormat="1">
+      <c r="A52" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B52" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C52" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="D52" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="E52" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="F52" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="G52" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="H52" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="I52" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="J52" s="28" t="s">
+        <v>57</v>
+      </c>
+      <c r="K52" s="28" t="s">
+        <v>59</v>
+      </c>
+      <c r="L52" s="28"/>
+      <c r="M52" s="28"/>
+      <c r="N52" s="28"/>
+    </row>
+    <row r="53" spans="1:14" s="4" customFormat="1" ht="51">
+      <c r="A53" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="B53" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D53" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E53" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F53" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="J10" s="5"/>
-      <c r="K10" s="5"/>
-      <c r="L10" s="5"/>
-      <c r="M10" s="5"/>
-      <c r="N10" s="5"/>
-    </row>
-    <row r="11" spans="1:14" s="7" customFormat="1">
-      <c r="A11" s="11" t="s">
+      <c r="G53" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="H53" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="I53" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="J53" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="K53" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="L53" s="10"/>
+      <c r="M53" s="10"/>
+      <c r="N53" s="10"/>
+    </row>
+    <row r="54" spans="1:14">
+      <c r="A54" s="21"/>
+    </row>
+    <row r="55" spans="1:14" s="6" customFormat="1">
+      <c r="A55" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="B55" s="5"/>
+      <c r="D55" s="5"/>
+      <c r="F55" s="5"/>
+      <c r="H55" s="5"/>
+      <c r="J55" s="5"/>
+      <c r="K55" s="5"/>
+      <c r="L55" s="5"/>
+      <c r="M55" s="5"/>
+      <c r="N55" s="5"/>
+    </row>
+    <row r="56" spans="1:14" s="7" customFormat="1">
+      <c r="A56" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B11" s="12" t="s">
+      <c r="B56" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="29" t="s">
+      <c r="C56" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="29" t="s">
+      <c r="D56" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="E11" s="29" t="s">
+      <c r="E56" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="F11" s="29" t="s">
+      <c r="F56" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="G11" s="29" t="s">
+      <c r="G56" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="H56" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="H11" s="29" t="s">
+      <c r="I56" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="J56" s="28" t="s">
+        <v>57</v>
+      </c>
+      <c r="K56" s="28" t="s">
+        <v>59</v>
+      </c>
+      <c r="L56" s="28"/>
+      <c r="M56" s="28"/>
+      <c r="N56" s="28"/>
+    </row>
+    <row r="57" spans="1:14" s="4" customFormat="1" ht="25.5">
+      <c r="A57" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="B57" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D57" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E57" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F57" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G57" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="H57" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="I57" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="J57" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="K57" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="L57" s="10"/>
+      <c r="M57" s="10"/>
+      <c r="N57" s="10"/>
+    </row>
+    <row r="58" spans="1:14">
+      <c r="A58" s="21"/>
+    </row>
+    <row r="59" spans="1:14" s="6" customFormat="1">
+      <c r="A59" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="B59" s="5"/>
+      <c r="D59" s="5"/>
+      <c r="F59" s="5"/>
+      <c r="H59" s="5"/>
+      <c r="J59" s="5"/>
+      <c r="K59" s="5"/>
+      <c r="L59" s="5"/>
+      <c r="M59" s="5"/>
+      <c r="N59" s="5"/>
+    </row>
+    <row r="60" spans="1:14" s="7" customFormat="1">
+      <c r="A60" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B60" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C60" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="D60" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="E60" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="F60" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="G60" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="I11" s="29" t="s">
+      <c r="H60" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="I60" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="J11" s="28"/>
-      <c r="K11" s="28"/>
-      <c r="L11" s="28"/>
-      <c r="M11" s="28"/>
-      <c r="N11" s="28"/>
-    </row>
-    <row r="12" spans="1:14" s="4" customFormat="1" ht="25.5">
-      <c r="A12" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="B12" s="14" t="s">
+      <c r="J60" s="28"/>
+      <c r="K60" s="28"/>
+      <c r="L60" s="28"/>
+      <c r="M60" s="28"/>
+      <c r="N60" s="28"/>
+    </row>
+    <row r="61" spans="1:14" s="4" customFormat="1" ht="25.5">
+      <c r="A61" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="B61" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="C61" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D12" s="4" t="s">
+      <c r="D61" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E12" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="H12" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="I12" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="J12" s="10"/>
-      <c r="K12" s="10"/>
-      <c r="L12" s="10"/>
-      <c r="M12" s="10"/>
-      <c r="N12" s="10"/>
-    </row>
-    <row r="13" spans="1:14">
-      <c r="A13" s="21"/>
+      <c r="E61" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F61" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G61" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="H61" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="I61" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="J61" s="10"/>
+      <c r="K61" s="10"/>
+      <c r="L61" s="10"/>
+      <c r="M61" s="10"/>
+      <c r="N61" s="10"/>
+    </row>
+    <row r="62" spans="1:14">
+      <c r="A62" s="21"/>
+    </row>
+    <row r="63" spans="1:14" s="6" customFormat="1">
+      <c r="A63" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="B63" s="5"/>
+      <c r="D63" s="5"/>
+      <c r="F63" s="5"/>
+      <c r="H63" s="5"/>
+      <c r="J63" s="5"/>
+      <c r="K63" s="5"/>
+      <c r="L63" s="5"/>
+      <c r="M63" s="5"/>
+      <c r="N63" s="5"/>
+    </row>
+    <row r="64" spans="1:14" s="7" customFormat="1">
+      <c r="A64" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B64" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C64" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="D64" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="E64" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="F64" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="G64" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="H64" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="I64" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="J64" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="K64" s="28"/>
+      <c r="L64" s="28"/>
+      <c r="M64" s="28"/>
+      <c r="N64" s="28"/>
+    </row>
+    <row r="65" spans="1:14" s="4" customFormat="1" ht="25.5">
+      <c r="A65" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="B65" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C65" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D65" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E65" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F65" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G65" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="H65" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="I65" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="J65" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="K65" s="10"/>
+      <c r="L65" s="10"/>
+      <c r="M65" s="10"/>
+      <c r="N65" s="10"/>
+    </row>
+    <row r="66" spans="1:14">
+      <c r="A66" s="21"/>
+    </row>
+    <row r="67" spans="1:14" s="6" customFormat="1">
+      <c r="A67" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="B67" s="5"/>
+      <c r="D67" s="5"/>
+      <c r="F67" s="5"/>
+      <c r="H67" s="5"/>
+      <c r="J67" s="5"/>
+      <c r="K67" s="5"/>
+      <c r="L67" s="5"/>
+      <c r="M67" s="5"/>
+      <c r="N67" s="5"/>
+    </row>
+    <row r="68" spans="1:14" s="7" customFormat="1">
+      <c r="A68" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B68" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C68" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="D68" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="E68" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="F68" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="G68" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="H68" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="I68" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="J68" s="28"/>
+      <c r="K68" s="28"/>
+      <c r="L68" s="28"/>
+      <c r="M68" s="28"/>
+      <c r="N68" s="28"/>
+    </row>
+    <row r="69" spans="1:14" s="4" customFormat="1" ht="25.5">
+      <c r="A69" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="B69" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="C69" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D69" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E69" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F69" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="G69" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="H69" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="I69" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="J69" s="10"/>
+      <c r="K69" s="10"/>
+      <c r="L69" s="10"/>
+      <c r="M69" s="10"/>
+      <c r="N69" s="10"/>
+    </row>
+    <row r="70" spans="1:14">
+      <c r="A70" s="21"/>
+    </row>
+    <row r="71" spans="1:14" s="6" customFormat="1">
+      <c r="A71" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="B71" s="5"/>
+      <c r="D71" s="5"/>
+      <c r="F71" s="5"/>
+      <c r="H71" s="5"/>
+      <c r="J71" s="5"/>
+      <c r="K71" s="5"/>
+      <c r="L71" s="5"/>
+      <c r="M71" s="5"/>
+      <c r="N71" s="5"/>
+    </row>
+    <row r="72" spans="1:14" s="7" customFormat="1">
+      <c r="A72" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B72" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C72" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="D72" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="E72" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="F72" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="G72" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="H72" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="I72" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="J72" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="K72" s="28"/>
+      <c r="L72" s="28"/>
+      <c r="M72" s="28"/>
+      <c r="N72" s="28"/>
+    </row>
+    <row r="73" spans="1:14" s="4" customFormat="1" ht="25.5">
+      <c r="A73" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="B73" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="C73" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D73" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E73" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F73" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="G73" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="H73" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="I73" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="J73" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="K73" s="10"/>
+      <c r="L73" s="10"/>
+      <c r="M73" s="10"/>
+      <c r="N73" s="10"/>
+    </row>
+    <row r="74" spans="1:14">
+      <c r="A74" s="21"/>
+    </row>
+    <row r="75" spans="1:14" s="6" customFormat="1">
+      <c r="A75" s="27" t="s">
+        <v>70</v>
+      </c>
+      <c r="B75" s="5"/>
+      <c r="D75" s="5"/>
+      <c r="F75" s="5"/>
+      <c r="H75" s="5"/>
+      <c r="J75" s="5"/>
+      <c r="K75" s="5"/>
+      <c r="L75" s="5"/>
+      <c r="M75" s="5"/>
+      <c r="N75" s="5"/>
+    </row>
+    <row r="76" spans="1:14" s="7" customFormat="1">
+      <c r="A76" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B76" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C76" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="D76" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="E76" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="F76" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="G76" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="H76" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="I76" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="J76" s="28"/>
+      <c r="K76" s="28"/>
+      <c r="L76" s="28"/>
+      <c r="M76" s="28"/>
+      <c r="N76" s="28"/>
+    </row>
+    <row r="77" spans="1:14" s="4" customFormat="1" ht="25.5">
+      <c r="A77" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="B77" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="C77" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D77" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E77" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F77" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="G77" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="H77" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="I77" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="J77" s="10"/>
+      <c r="K77" s="10"/>
+      <c r="L77" s="10"/>
+      <c r="M77" s="10"/>
+      <c r="N77" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>